<commit_message>
Publication year evolution of the included records
</commit_message>
<xml_diff>
--- a/data/results/analysis.xlsx
+++ b/data/results/analysis.xlsx
@@ -8,14 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C0FA4-A441-4FB1-8EF0-CE1A2B673EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB4CB38-6F70-4A0C-AC0C-0DF0E041605C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="included" sheetId="1" r:id="rId1"/>
     <sheet name="analysis-db" sheetId="2" r:id="rId2"/>
+    <sheet name="year" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'analysis-db'!$B$2:$B$145</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">[1]Analysis!$C$2:$C$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">[1]Analysis!$D$2:$D$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="596">
   <si>
     <t>author</t>
   </si>
@@ -1826,6 +1835,12 @@
   </si>
   <si>
     <t>ok so, indeed, searching the query on inspec, scopus and wos led to obtaining all the results included in the review</t>
+  </si>
+  <si>
+    <t>#records</t>
+  </si>
+  <si>
+    <t>Evolution of the year of publication relative to the included records in the review</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1848,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1917,7 +1932,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2094,6 +2109,1327 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Evolution of the publication year</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>year!$A$2:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2022</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>year!$B$2:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FE3A-449E-89D7-92B3FB237278}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1562487728"/>
+        <c:axId val="1562488144"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1562487728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2022"/>
+          <c:min val="2002"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>year</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1562488144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1562488144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>#records</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1562487728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A6214F2-4468-4259-805A-7F4BB80711DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Eligible Records"/>
+      <sheetName val="Parsifal QE"/>
+      <sheetName val="Analysis"/>
+      <sheetName val="Graphs Analysis"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2">
+        <row r="2">
+          <cell r="C2">
+            <v>0</v>
+          </cell>
+          <cell r="D2">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="C3">
+            <v>0.5</v>
+          </cell>
+          <cell r="D3">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>1</v>
+          </cell>
+          <cell r="D4">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>1.5</v>
+          </cell>
+          <cell r="D5">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="C6">
+            <v>2</v>
+          </cell>
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>2.5</v>
+          </cell>
+          <cell r="D7">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>3</v>
+          </cell>
+          <cell r="D8">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="C9">
+            <v>3.5</v>
+          </cell>
+          <cell r="D9">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="C10">
+            <v>4</v>
+          </cell>
+          <cell r="D10">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>4.5</v>
+          </cell>
+          <cell r="D11">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>5</v>
+          </cell>
+          <cell r="D12">
+            <v>18</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="C13">
+            <v>5.5</v>
+          </cell>
+          <cell r="D13">
+            <v>21</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="C14">
+            <v>6</v>
+          </cell>
+          <cell r="D14">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="C15">
+            <v>6.5</v>
+          </cell>
+          <cell r="D15">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="C16">
+            <v>7</v>
+          </cell>
+          <cell r="D16">
+            <v>51</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="C17">
+            <v>7.5</v>
+          </cell>
+          <cell r="D17">
+            <v>68</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="C18">
+            <v>8</v>
+          </cell>
+          <cell r="D18">
+            <v>41</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="C19">
+            <v>8.5</v>
+          </cell>
+          <cell r="D19">
+            <v>43</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="C20">
+            <v>9</v>
+          </cell>
+          <cell r="D20">
+            <v>56</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="C21">
+            <v>9.5</v>
+          </cell>
+          <cell r="D21">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="C22">
+            <v>10</v>
+          </cell>
+          <cell r="D22">
+            <v>21</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4951,7 +6287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A8216EB-1D21-4E7E-9A29-BD466C104F0E}">
   <dimension ref="A1:Q146"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A105" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6177,7 +7513,7 @@
         <v>121</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" ref="O27:Q28" si="0">SUM($E$2:$E$145)+SUM(H$2:H$145)-SUMPRODUCT($E$2:$E$145,H$2:H$145)</f>
+        <f t="shared" ref="P28:Q28" si="0">SUM($E$2:$E$145)+SUM(H$2:H$145)-SUMPRODUCT($E$2:$E$145,H$2:H$145)</f>
         <v>124</v>
       </c>
       <c r="Q28" s="1">
@@ -6230,7 +7566,7 @@
         <v>109</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" ref="P28:Q29" si="1">SUM($F$2:$F$145)+SUM(H$2:H$145)-SUMPRODUCT($F$2:$F$145,H$2:H$145)</f>
+        <f t="shared" ref="P29" si="1">SUM($F$2:$F$145)+SUM(H$2:H$145)-SUMPRODUCT($F$2:$F$145,H$2:H$145)</f>
         <v>128</v>
       </c>
       <c r="Q29" s="1">
@@ -6567,7 +7903,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="O36" s="12">
-        <f t="shared" ref="O35:Q36" si="2">(SUM($E$2:$E$145)+SUM(G$2:G$145)-SUMPRODUCT($E$2:$E$145,G$2:G$145))/COUNTIF($A$2:$A$145,"&lt;&gt;")</f>
+        <f t="shared" ref="O36:Q36" si="2">(SUM($E$2:$E$145)+SUM(G$2:G$145)-SUMPRODUCT($E$2:$E$145,G$2:G$145))/COUNTIF($A$2:$A$145,"&lt;&gt;")</f>
         <v>0.84027777777777779</v>
       </c>
       <c r="P36" s="12">
@@ -6624,7 +7960,7 @@
         <v>0.75694444444444442</v>
       </c>
       <c r="P37" s="12">
-        <f t="shared" ref="P36:Q37" si="3">(SUM($F$2:$F$145)+SUM(H$2:H$145)-SUMPRODUCT($F$2:$F$145,H$2:H$145))/COUNTIF($A$2:$A$145,"&lt;&gt;")</f>
+        <f t="shared" ref="P37:Q37" si="3">(SUM($F$2:$F$145)+SUM(H$2:H$145)-SUMPRODUCT($F$2:$F$145,H$2:H$145))/COUNTIF($A$2:$A$145,"&lt;&gt;")</f>
         <v>0.88888888888888884</v>
       </c>
       <c r="Q37" s="12">
@@ -9851,27 +11187,27 @@
         <v>582</v>
       </c>
       <c r="D146" s="10">
-        <f>SUM(D2:D145)</f>
+        <f t="shared" ref="D146:I146" si="4">SUM(D2:D145)</f>
         <v>0</v>
       </c>
       <c r="E146" s="10">
-        <f>SUM(E2:E145)</f>
+        <f t="shared" si="4"/>
         <v>65</v>
       </c>
       <c r="F146" s="10">
-        <f>SUM(F2:F145)</f>
+        <f t="shared" si="4"/>
         <v>67</v>
       </c>
       <c r="G146" s="10">
-        <f>SUM(G2:G145)</f>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="H146" s="10">
-        <f>SUM(H2:H145)</f>
+        <f t="shared" si="4"/>
         <v>122</v>
       </c>
       <c r="I146" s="10">
-        <f>SUM(I2:I145)</f>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
       <c r="J146" s="1">
@@ -9882,6 +11218,247 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07199B29-2ED9-434A-B4E7-BF2498275BB9}">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="4.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <f>MIN(included[year])</f>
+        <v>2002</v>
+      </c>
+      <c r="B2" s="1">
+        <f>COUNTIF(included[year],A2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <f>A2+1</f>
+        <v>2003</v>
+      </c>
+      <c r="B3" s="1">
+        <f>COUNTIF(included[year],A3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A35" si="0">A3+1</f>
+        <v>2004</v>
+      </c>
+      <c r="B4" s="1">
+        <f>COUNTIF(included[year],A4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>2005</v>
+      </c>
+      <c r="B5" s="1">
+        <f>COUNTIF(included[year],A5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>2006</v>
+      </c>
+      <c r="B6" s="1">
+        <f>COUNTIF(included[year],A6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>2007</v>
+      </c>
+      <c r="B7" s="1">
+        <f>COUNTIF(included[year],A7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>2008</v>
+      </c>
+      <c r="B8" s="1">
+        <f>COUNTIF(included[year],A8)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>2009</v>
+      </c>
+      <c r="B9" s="1">
+        <f>COUNTIF(included[year],A9)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>2010</v>
+      </c>
+      <c r="B10" s="1">
+        <f>COUNTIF(included[year],A10)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>2011</v>
+      </c>
+      <c r="B11" s="1">
+        <f>COUNTIF(included[year],A11)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>2012</v>
+      </c>
+      <c r="B12" s="1">
+        <f>COUNTIF(included[year],A12)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>2013</v>
+      </c>
+      <c r="B13" s="1">
+        <f>COUNTIF(included[year],A13)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>2014</v>
+      </c>
+      <c r="B14" s="1">
+        <f>COUNTIF(included[year],A14)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>2015</v>
+      </c>
+      <c r="B15" s="1">
+        <f>COUNTIF(included[year],A15)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>2016</v>
+      </c>
+      <c r="B16" s="1">
+        <f>COUNTIF(included[year],A16)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>2017</v>
+      </c>
+      <c r="B17" s="1">
+        <f>COUNTIF(included[year],A17)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>2018</v>
+      </c>
+      <c r="B18" s="1">
+        <f>COUNTIF(included[year],A18)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>2019</v>
+      </c>
+      <c r="B19" s="1">
+        <f>COUNTIF(included[year],A19)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>2020</v>
+      </c>
+      <c r="B20" s="1">
+        <f>COUNTIF(included[year],A20)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>2021</v>
+      </c>
+      <c r="B21" s="1">
+        <f>COUNTIF(included[year],A21)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="B22" s="1">
+        <f>COUNTIF(included[year],A22)</f>
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Minor dev venues analysis
</commit_message>
<xml_diff>
--- a/data/results/analysis.xlsx
+++ b/data/results/analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDE7B5A-4BB9-40F2-9BFD-32F8E6226FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCAAB3F-1C4C-43BB-A7C5-0A495707B875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="included" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2046" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="874">
   <si>
     <t>author</t>
   </si>
@@ -2701,7 +2701,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="174" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -2760,7 +2760,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2795,134 +2795,16 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="48">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="174" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2949,6 +2831,45 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3005,6 +2926,133 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -3025,7 +3073,25 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -3117,7 +3183,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3156,76 +3221,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3518,6 +3514,13 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -4918,80 +4921,80 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B29708E5-A0F6-4F6B-88B6-E4684ADDD699}" name="venue" displayName="venue" ref="A1:H145" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B29708E5-A0F6-4F6B-88B6-E4684ADDD699}" name="venue" displayName="venue" ref="A1:H145" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:H145" xr:uid="{B29708E5-A0F6-4F6B-88B6-E4684ADDD699}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H145">
     <sortCondition ref="G2:G145"/>
     <sortCondition ref="D2:D145"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{66758D5A-C3D8-46E0-97ED-2777D2EABE61}" name="type" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{FA49994D-FED8-40DA-AC2D-5F4F33460CBE}" name="title" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{4F3DA2DC-DB8D-4E6A-BC21-6D14234535DE}" name="authors" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{E832F53F-A13B-4916-8145-1BAD7CCF4B25}" name="year" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{B4205B62-8EBC-48B8-9A3C-2D019B57F085}" name="doi" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{82087277-E247-4CF7-B2A2-A32929A2BDF5}" name="url" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{C0DBEEF9-37B7-4B16-A674-42707F8457DD}" name="venue" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{425564B3-8374-4756-99CB-DA71938972EE}" name="active?" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{66758D5A-C3D8-46E0-97ED-2777D2EABE61}" name="type" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{FA49994D-FED8-40DA-AC2D-5F4F33460CBE}" name="title" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{4F3DA2DC-DB8D-4E6A-BC21-6D14234535DE}" name="authors" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{E832F53F-A13B-4916-8145-1BAD7CCF4B25}" name="year" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{B4205B62-8EBC-48B8-9A3C-2D019B57F085}" name="doi" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{82087277-E247-4CF7-B2A2-A32929A2BDF5}" name="url" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{C0DBEEF9-37B7-4B16-A674-42707F8457DD}" name="venue" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{425564B3-8374-4756-99CB-DA71938972EE}" name="active?" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BFFB38C-40F9-478D-A54A-A7AC121E0B1E}" name="venue_all" displayName="venue_all" ref="L4:R44" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4BFFB38C-40F9-478D-A54A-A7AC121E0B1E}" name="venue_all" displayName="venue_all" ref="L4:R44" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="L4:R44" xr:uid="{4BFFB38C-40F9-478D-A54A-A7AC121E0B1E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L5:R44">
     <sortCondition ref="L4:L44"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{ECE705E8-471D-4354-A829-0795DDCA413C}" name="unique venue" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{0450DD41-9669-4D5C-9EA9-6930DEC7B864}" name="med year" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{ECE705E8-471D-4354-A829-0795DDCA413C}" name="unique venue" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{0450DD41-9669-4D5C-9EA9-6930DEC7B864}" name="med year" dataDxfId="26">
       <calculatedColumnFormula array="1">MEDIAN(IF(venue[venue]=venue_all[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{AC3DB23C-6718-49F4-9AFC-0E0C691A22B4}" name="max year" dataDxfId="26">
+    <tableColumn id="6" xr3:uid="{AC3DB23C-6718-49F4-9AFC-0E0C691A22B4}" name="max year" dataDxfId="25">
       <calculatedColumnFormula array="1">MAX(IF(venue[venue]=venue_all[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{63BFA84C-CFCF-46CA-B157-FADCC0D3A739}" name="std" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{63BFA84C-CFCF-46CA-B157-FADCC0D3A739}" name="std" dataDxfId="24">
       <calculatedColumnFormula array="1">_xlfn.STDEV.P(IF(venue[venue]=venue_all[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B6FCD29F-9EA3-4B29-8344-C366D7A01FAC}" name="#records" dataDxfId="25">
+    <tableColumn id="2" xr3:uid="{B6FCD29F-9EA3-4B29-8344-C366D7A01FAC}" name="#records" dataDxfId="23">
       <calculatedColumnFormula>COUNTIF(venue[venue],venue_all[[#This Row],[unique venue]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F78F36C9-68A1-4D30-BA97-F1E79A2635E6}" name="avg year" dataDxfId="24">
+    <tableColumn id="3" xr3:uid="{F78F36C9-68A1-4D30-BA97-F1E79A2635E6}" name="avg year" dataDxfId="22">
       <calculatedColumnFormula>AVERAGEIF(venue[venue],venue_all[[#This Row],[unique venue]],venue[year])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{1B18FA27-8DC9-41D7-8DB5-6B00D35A7C53}" name="active?" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{1B18FA27-8DC9-41D7-8DB5-6B00D35A7C53}" name="active?" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0EB9D00F-6515-4F06-967B-2F32D29BB1DE}" name="venue_conf" displayName="venue_conf" ref="L51:R66" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0EB9D00F-6515-4F06-967B-2F32D29BB1DE}" name="venue_conf" displayName="venue_conf" ref="L51:R66" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="L51:R66" xr:uid="{0EB9D00F-6515-4F06-967B-2F32D29BB1DE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L52:R66">
     <sortCondition descending="1" ref="R52:R66"/>
     <sortCondition descending="1" ref="Q52:Q66"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{0AE5386B-B649-46C7-A34B-45EB60AED0E1}" name="unique venue" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{2938F512-0A83-471C-B390-C0FABAAAAB81}" name="avg year" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{0AE5386B-B649-46C7-A34B-45EB60AED0E1}" name="unique venue" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{2938F512-0A83-471C-B390-C0FABAAAAB81}" name="avg year" dataDxfId="8">
       <calculatedColumnFormula>AVERAGEIF(venue[venue],venue_conf[[#This Row],[unique venue]],venue[year])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{04AA019A-43C1-4D41-AEF2-8FFD77EF8398}" name="std" dataDxfId="3">
+    <tableColumn id="7" xr3:uid="{04AA019A-43C1-4D41-AEF2-8FFD77EF8398}" name="std" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn.STDEV.P(IF(venue[venue]=venue_conf[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0E5B15F9-EEAF-4CE7-AB2A-2113F2E1ED7D}" name="max year" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{0E5B15F9-EEAF-4CE7-AB2A-2113F2E1ED7D}" name="max year" dataDxfId="6">
       <calculatedColumnFormula array="1">MAX(IF(venue[venue]=venue_conf[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6843392C-CBCF-45F8-8989-16C4AA20F28D}" name="#records" dataDxfId="10">
+    <tableColumn id="2" xr3:uid="{6843392C-CBCF-45F8-8989-16C4AA20F28D}" name="#records" dataDxfId="5">
       <calculatedColumnFormula>COUNTIF(venue[venue],venue_conf[[#This Row],[unique venue]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{EEC30FBE-687D-46C8-858B-5637FC211AE1}" name="med year" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{EEC30FBE-687D-46C8-858B-5637FC211AE1}" name="med year" dataDxfId="4">
       <calculatedColumnFormula array="1">MEDIAN(IF(venue[venue]=venue_conf[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{33E922CC-1BF4-4BC0-AF69-5D16B1BF1E78}" name="active?" dataDxfId="18">
+    <tableColumn id="4" xr3:uid="{33E922CC-1BF4-4BC0-AF69-5D16B1BF1E78}" name="active?" dataDxfId="3">
       <calculatedColumnFormula>LOOKUP(venue_conf[[#This Row],[unique venue]],venue_all[unique venue],venue_all[active?])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5000,30 +5003,30 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{ABC89EDF-F1D8-46DA-929F-82A916BA7F02}" name="venue_journal" displayName="venue_journal" ref="L73:R98" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{ABC89EDF-F1D8-46DA-929F-82A916BA7F02}" name="venue_journal" displayName="venue_journal" ref="L73:R98" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="L73:R98" xr:uid="{ABC89EDF-F1D8-46DA-929F-82A916BA7F02}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L74:R98">
     <sortCondition descending="1" ref="R74:R98"/>
     <sortCondition descending="1" ref="Q74:Q98"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D2FDEA0A-90F1-4B25-B56B-9964A6536388}" name="unique venue" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{E7CAF3BD-66FB-4438-9454-F0D305D98F04}" name="avg year" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{D2FDEA0A-90F1-4B25-B56B-9964A6536388}" name="unique venue" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{E7CAF3BD-66FB-4438-9454-F0D305D98F04}" name="avg year" dataDxfId="17">
       <calculatedColumnFormula>AVERAGEIF(venue[venue],venue_journal[[#This Row],[unique venue]],venue[year])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{23477729-9500-45BE-B263-E09F8E84A798}" name="std" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{23477729-9500-45BE-B263-E09F8E84A798}" name="std" dataDxfId="16">
       <calculatedColumnFormula array="1">_xlfn.STDEV.P(IF(venue[venue]=venue_journal[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3C7312C7-EC50-4132-8D8A-E8ECCDA520E7}" name="max year" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{3C7312C7-EC50-4132-8D8A-E8ECCDA520E7}" name="max year" dataDxfId="15">
       <calculatedColumnFormula array="1">MAX(IF(venue[venue]=venue_journal[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{1E45BF40-82D1-4A03-8017-A6B337DDEF0D}" name="#records" dataDxfId="11">
+    <tableColumn id="2" xr3:uid="{1E45BF40-82D1-4A03-8017-A6B337DDEF0D}" name="#records" dataDxfId="14">
       <calculatedColumnFormula>COUNTIF(venue[venue],venue_journal[[#This Row],[unique venue]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0E8372DD-39C7-4D91-B944-E7ED984DAFC9}" name="med year" dataDxfId="14">
+    <tableColumn id="5" xr3:uid="{0E8372DD-39C7-4D91-B944-E7ED984DAFC9}" name="med year" dataDxfId="13">
       <calculatedColumnFormula array="1">MEDIAN(IF(venue[venue]=venue_journal[[#This Row],[unique venue]],venue[year]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{FC9A04E1-F4AC-4287-A35A-7C9397044171}" name="active?" dataDxfId="13">
+    <tableColumn id="4" xr3:uid="{FC9A04E1-F4AC-4287-A35A-7C9397044171}" name="active?" dataDxfId="12">
       <calculatedColumnFormula>LOOKUP(venue_journal[[#This Row],[unique venue]],venue_all[unique venue],venue_all[active?])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -13069,7 +13072,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2D9B05-43B4-48AE-95C7-898F4F58C07D}">
   <dimension ref="A1:R145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q67" sqref="Q67"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16313,6 +16318,28 @@
       <c r="G67" s="1" t="s">
         <v>608</v>
       </c>
+      <c r="L67" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="M67" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="P67" s="1">
+        <f>SUM(venue_conf['#records])</f>
+        <v>62</v>
+      </c>
+      <c r="Q67" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
@@ -17830,6 +17857,28 @@
       <c r="G99" s="1" t="s">
         <v>855</v>
       </c>
+      <c r="L99" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="M99" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="N99" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="P99" s="1">
+        <f>SUM(venue_journal['#records])</f>
+        <v>82</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
@@ -18890,21 +18939,21 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O2:O3 R4:R44 O99:O145 R73:R98 O45:O50 O67:O72 R51:R66">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="no">
+  <conditionalFormatting sqref="O2:O3 R4:R44 R73:R98 O45:O50 O67:O72 R51:R66 O99:O145">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="no">
       <formula>NOT(ISERROR(SEARCH("no",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="yes">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="yes">
       <formula>NOT(ISERROR(SEARCH("yes",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:M44 Q5:Q44">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="40" priority="8">
       <formula>($Q5=$M5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M74:M98 Q74:Q98 M52:M66 Q52:Q66">
-    <cfRule type="expression" dxfId="6" priority="13">
+    <cfRule type="expression" dxfId="0" priority="13">
       <formula>($M52=$Q52)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>